<commit_message>
Zeitblatter auf stand gebracht
</commit_message>
<xml_diff>
--- a/Zeitblätter/Ursus Schneider.xlsx
+++ b/Zeitblätter/Ursus Schneider.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>10:45 - 11:15</t>
+  </si>
+  <si>
+    <t>DMX und ESP ferigstellen</t>
+  </si>
+  <si>
+    <t>DMX und ESP weitere arbeit</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00</t>
+  </si>
+  <si>
+    <t>14:00 - 16:00</t>
   </si>
 </sst>
 </file>
@@ -471,7 +483,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,11 +767,29 @@
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42667</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,7 +843,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B5:B34)</f>
-        <v>36.75</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>